<commit_message>
leiaute; tenta fazer referencia virar componente
</commit_message>
<xml_diff>
--- a/docs/Noticias/Resumo votações na Câmara.xlsx
+++ b/docs/Noticias/Resumo votações na Câmara.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dados\Tecnicos\HardESoftware\EmDesenvolvimento\VotoBomPython\django_votebem\docs\Noticias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F76555-7EA4-4916-8A01-7D116D9BCF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F228F416-87CC-4A38-8BE7-70630A341FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{53B4B6C9-9AD8-4847-8B7A-A3110067C019}"/>
   </bookViews>
@@ -2519,6 +2519,1732 @@
   </si>
   <si>
     <r>
+      <t>Pena para Imagens de Nudez Geradas por IA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Aprovado o projeto de lei que inclui no Código Penal o crime de manipular, produzir ou divulgar conteúdo de nudez ou ato sexual falso gerado por inteligência artificial,. O crime pode ser punido com reclusão de dois a seis anos e multa, com aumento de pena se a vítima for mulher, criança ou idosa.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Reajuste dos Servidores Públicos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Aprovado o reajuste para servidores públicos (388 a 43 votos), garantindo um impacto de R$ 17,9 bilhões em 2025 para os aumentos salariais,. A discussão sobre a reestruturação de carreiras (Sidec) foi postergada para um grupo de trabalho,,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pauta-Bomba de Crédito Subsidiado para o Agronegócio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Aprovado (346 a 93) um projeto que inclui um crédito subsidiado de até R$ 30 bilhões para o agronegócio, usando verbas do Fundo Social do pré-sal,,. A votação ocorreu em um clima de retaliação após decisões desfavoráveis do Executivo e Judiciário,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Flexibilização do Licenciamento Ambiental</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Aprovado o projeto (267 a 116) que flexibiliza e simplifica o licenciamento ambiental, mantendo mecanismos criticados por ambientalistas, como a Licença Ambiental Especial (LAE),,,. O texto, que segue para sanção presidencial, é visto como um impulso para projetos como a exploração de petróleo na Foz do Amazonas,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Proteção de Crianças e Adolescentes no Ambiente Digital</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Aprovado simbolicamente (apenas Novo e um deputado votaram contra) o projeto que visa proteger crianças e adolescentes em meios digitais, exigindo que plataformas implementem mecanismos para impedir acesso a conteúdos inadequados,,. O texto segue para o Senado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Criação do Sistema Nacional de Educação ('SUS da Educação')</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Aprovado o projeto que institui o Sistema Nacional de Educação (SNE), buscando a cooperação técnica e financeira entre União, estados e municípios para políticas educacionais,,. O texto cria a Infraestrutura Nacional de Dados da Educação e o Identificador Nacional Único do Estudante.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Gratuidade de Bagagem e Marcação de Assento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Aprovada a gratuidade da bagagem despachada (361 a 77 votos) e de mão, além da proibição de cobrança pela marcação de assento padrão em voos nacionais ou internacionais,,. O projeto segue para o Senado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Medidas de Corte de Gastos e Atualização de Imóveis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Aprovado o projeto (286 a 146) que cria o Regime Especial de Atualização e Regularização Patrimonial (Rearp) de bens móveis e imóveis, com pagamento de alíquota menor de tributo,. O texto incluiu medidas de contenção de despesas do governo, com impacto fiscal estimado em R$ 15 bilhões,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Plano Nacional do Esporte (PNEsporte)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, previsto na Lei Pelé, que estabelece princípios e objetivos para o esporte brasileiro,,. O texto proíbe o contingenciamento de recursos destinados ao esporte provenientes da arrecadação das loterias federais,. A votação foi simbólica e a proposta seguiu para o Senado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foi aprovada uma Medida Provisória (MP) que autoriza a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>concessão de empréstimo consignado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para beneficiários do Auxílio Brasil e do BPC (Benefício de Prestação Continuada),. O limite de contratação de crédito consignado para esses beneficiários é de 40% do valor do benefício,. O texto-base foi aprovado por 245 votos a 69.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou uma MP para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reduzir as filas do INSS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, permitindo a concessão de auxílio por incapacidade temporária (o antigo auxílio-doença) sem perícia médica presencial,. A MP também inclui o auxílio-acidente no rol de benefícios que passarão por reavaliações e revisões periódicas,. O texto-base foi aprovado por 381 votos a 8.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foi aprovada uma Medida Provisória que autoriza o governo a adotar </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>medidas trabalhistas alternativas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (como teletrabalho facilitado e antecipação de férias) para mitigar as consequências sociais e econômicas de um estado de calamidade pública,. O texto-base foi aprovado por 249 votos a 111.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O texto-base da Medida Provisória que altera as regras sobre o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vale-alimentação</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> foi aprovado por 248 votos a 159,. Uma das principais mudanças mantidas permite que, após 60 dias sem uso, o saldo do vale-alimentação possa ser sacado pelo trabalhador.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foi aprovado o projeto que cria as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>loterias da Saúde e do Turismo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, permitindo a exploração dos novos jogos pela iniciativa privada,. Os recursos arrecadados serão destinados ao Fundo Nacional de Saúde (FNS) e à Embratur,. O texto foi aprovado por 267 a 94.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou em dois turnos uma PEC que permite a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reeleição para a direção dos Tribunais de Justiça (TJs)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> estaduais que possuem mais de 170 desembargadores, o que se aplica aos TJs de São Paulo e Rio de Janeiro,,. A inclusão da possibilidade de recondução foi acrescentada ao texto um dia antes da votação, sem debate em comissões.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou uma MP do governo Bolsonaro que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>afrouxa a proteção à Mata Atlântica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,. O texto, alterado pelo relator, flexibiliza o desmatamento de vegetação primária e secundária e retira a exigência de medidas compensatórias para supressão fora de Áreas de Preservação Permanente (APP),,. O plenário também aprovou uma outra MP que permite a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>comercialização de créditos de carbono</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> em concessões de unidades de conservação e florestas públicas,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O plenário aprovou o texto-base da MP que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reestrutura a Esplanada dos Ministérios</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, evitando uma derrota do governo Lula,. O texto amplia o número de ministérios para 37, mas o governo foi obrigado a ceder e aceitar a recriação da Funasa,. A aprovação teve 337 votos a favor e 125 contra.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou o projeto de lei que cria o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>programa Escola em Tempo Integral</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. A proposta, que segue ao Senado, prevê um investimento de R$ 2 bilhões em assistência financeira para 2023 e 2024, com o objetivo de viabilizar um milhão de novas matrículas,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O texto do projeto que prorroga a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>desoneração da folha de pagamento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para 17 setores da economia até 2027 foi aprovado, representando uma derrota dupla para o ministro Fernando Haddad (Fazenda),. O projeto também reduz a contribuição previdenciária de municípios,. Recebeu 430 votos favoráveis e 17 contrários.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Aprovado em votação simbólica o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PL do Desenrola Brasil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, que estabelece regras para o programa de renegociação de dívidas e prevê um limite para os juros do rotativo do cartão de crédito,,. Caso as instituições financeiras não apresentem um plano de taxa menor em 90 dias, a dívida será limitada ao dobro do montante original,,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou o projeto que libera </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R$ 13,9 bilhões em repasses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para estados e municípios em 2023,. O montante inclui R$ 10 bilhões antecipados da compensação por cortes no ICMS e reposição de perdas nos fundos de participação (FPM e FPE),. O texto-base foi aprovado por 349 votos a 68.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O Congresso Nacional aprovou uma série de projetos para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>realocar recursos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> entre ministérios, com o objetivo de aumentar verbas para pastas e projetos ligados ao centrão e vitaminar as emendas parlamentares,. O Ministério das Cidades e o do Desenvolvimento Social perderam recursos em favor de órgãos como Codevasf,,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prorrogação da Lei Paulo Gustavo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> até dezembro de 2024, que destina R$ 3,86 bilhões para o fomento de atividades culturais,. A proposta seguiu para sanção presidencial e foi aprovada por 326 votos a 84,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou um projeto de lei que cria um </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cadastro nacional para monitorar facções criminosas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, incluindo milícias,. O cadastro será atualizado com base em decisões judiciais transitadas em julgado (condenações definitivas) e as informações reunidas serão sigilosas,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foi aprovado o projeto de lei que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>criminaliza a violação, adulteração ou troca de bagagem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de passageiros de avião ou ônibus para fins de tráfico de drogas,. O crime terá pena de 5 a 15 anos, que pode ser aumentada se o agente for funcionário do serviço de transporte,. A votação foi simbólica.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou, de forma simbólica, um projeto de lei que cria uma </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>política de acolhimento de animais resgatados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> durante desastres naturais,. A proposta prevê que municípios organizem sistemas de resgate e abrigos temporários, com equipes treinadas e avaliação veterinária imediata,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Em votação simbólica, foi aprovado o projeto de lei conhecido como "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lei Larissa Manoela</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", que insere no ECA (Estatuto da Criança e do Adolescente) o direito à proteção contra condutas abusivas na gestão patrimonial de crianças e adolescentes,,. O texto permite que um juiz determine restrições de acesso dos pais aos recursos ou a criação de uma reserva especial.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou um projeto que prorroga </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>benefícios tributários para o setor audiovisual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (como o Recine e a Lei do Audiovisual) e autoriza a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>redução de repasses da Lei Aldir Blanc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a estados e municípios que possuírem recursos não utilizados do ano anterior,,,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foi aprovado o projeto de lei complementar que visa aumentar o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>número de deputados federais de 513 para 531</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,. O aumento cria 18 novas cadeiras para redistribuir a representação dos estados de acordo com o Censo 2022, evitando que algumas bancadas perdessem assentos,. O placar foi de 270 a favor e 207 contra.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou projeto de lei que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aumenta as penas para crimes contra profissionais de saúde</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,. A proposta transforma em homicídio qualificado o assassinato desses profissionais no exercício da função (pena de 12 a 30 anos) e inclui lesão corporal contra eles no Código Penal (pena de 2 a 5 anos de prisão),. O texto foi aprovado por 310 votos contra 105.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foi aprovado o projeto que institui a chamada </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Lei do Mar"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, estabelecendo a Política Nacional para a Gestão Integrada, a Conservação e o Uso Sustentável do Sistema Costeiro-Marinho (PNGCMar),. O texto foi aprovado com 376 votos a favor e 66 contrários após 12 anos de discussão.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>derrubada dos decretos do governo que aumentavam as alíquotas do IOF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Imposto sobre Operações Financeiras). A medida foi aprovada por 383 votos a 98.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Em votação a jato, a Câmara aprovou a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>redação final do projeto que aumenta o número de deputados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de 513 para 531, incorporando alterações feitas pelo Senado,. As alterações incluíram uma restrição que proíbe qualquer aumento de despesa devido à criação das 18 novas cadeiras,. As mudanças tiveram o voto favorável de 361 deputados, contra 33.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou o projeto de lei que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dificulta a progressão de pena</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para condenados por crimes hediondos (como estupro e homicídio), exigindo o cumprimento de, no mínimo, 80% da pena,,. A regra também se aplica a sentenciados por constituir milícia privada ou exercer comando em organização criminosa.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Em dois turnos (446 a 20 e 426 a 10), a Câmara aprovou uma PEC que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>afrouxa as regras de aposentadoria para agentes comunitários de saúde e de combate a endemias</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,,. A medida, apelidada de "contrarreforma da Previdência", restabelece a integralidade e a paridade para a categoria, com um potencial impacto bilionário (estimado entre R$ 20 bilhões e R$ 200 bilhões) nas contas da União,,,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foi aprovado um pacote de 16 projetos relacionados à infância e educação. Entre eles, um projeto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aumenta a pena para pedófilos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (ex: estupro de vulnerável de 8-15 para 10-18 anos) e outro exige </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>autorização judicial para a atividade de influenciadores mirins</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou dois projetos propostos pelo STF para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aumentar os salários dos servidores do Poder Judiciário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> da União,. Um reajusta em 25,97% os vencimentos (escalonado até 2028), com 299 votos a 119. O outro, aprovado simbolicamente, ajusta o adicional de qualificação baseado em cursos e pós-graduação.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ratificação do Acordo de Escazú</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, um tratado internacional sobre transparência, participação pública, segurança e justiça em temas ambientais,. O acordo estava engavetado há seis anos e foi aprovado na véspera da COP30,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou um projeto de lei que institui a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Política Nacional de Saúde Masculina no SUS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, com foco em prevenção, detecção precoce e tratamento de doenças que acometem os homens,. O texto também implementa a campanha Novembro Azul em nível nacional.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou a versão do relator Guilherme Derrite (PP-SP) para o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PL Antifacção</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, em uma derrota para o governo Lula que tentava adiar a apreciação,. O projeto cria novos tipos penais, como Domínio Social Estruturado, para endurecer a punição contra organizações criminosas ultraviolentas,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou o projeto de lei que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prorroga a lei de cotas para negros em concursos públicos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,. O texto aumenta a reserva de vagas de 20% para 30% e inclui indígenas e quilombolas entre os beneficiados, mas precisará retornar ao Senado devido às alterações,,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou a MP que liberou </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>crédito extraordinário de R$ 12 bilhões</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para ações de socorro ao Rio Grande do Sul em decorrência das enchentes,. O texto foi aprovado com 257 votos favoráveis e 150 contrários.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foi aprovada a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lei Geral do Turismo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, retirando o trecho polêmico que limitaria a indenização a passageiros de companhias aéreas,,. O texto permite, entre outras coisas, a reabertura de empréstimos garantidos pelo Fundo Nacional da Aviação Civil (Fnac) para companhias aéreas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou uma alteração na </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lei de Responsabilidade Fiscal (LRF)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que flexibiliza os limites de gasto com pessoal de estados e municípios,. A mudança permite descontar do cálculo de despesa com pessoal os gastos com terceirização e organizações da sociedade civil,. A proposta foi aprovada por 370 votos favoráveis contra 15.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou um projeto que dá maior </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fôlego orçamentário a hospitais universitários</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. A medida exclui despesas de pessoal desses hospitais do cálculo para o cumprimento do limite constitucional mínimo de aplicação anual em saúde pública,. O texto será enviado à sanção presidencial.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara concluiu a votação e aprovou a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>desoneração da folha de pagamento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para 17 setores e municípios, após impasse com o Banco Central,. O projeto, aprovado por 253 votos a favor, mantém o benefício em 2024 e estabelece uma reoneração gradual entre 2025 e 2027,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou o projeto de lei que exige que as empresas aéreas </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ofereçam o serviço de rastreamento de animais de estimação (pets)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> transportados em voos domésticos,,. A proposta, aprovada de forma simbólica, surge após a morte do cão Joca,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foi aprovado o projeto de lei que cria </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R$ 18,3 bilhões em subsídios fiscais para projetos de hidrogênio verde</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,. O texto, que segue para o Senado, foi negociado após um veto anterior do presidente Lula, e concede crédito fiscal por meio da Contribuição Social sobre o Lucro Líquido (CSLL),,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Câmara aprovou, em dois turnos (344 a 89 e 338 a 83), a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PEC da Anistia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. A proposta revoga a obrigatoriedade de distribuir verba eleitoral de forma proporcional ao número de candidatos negros (pretos e pardos), fixando um mínimo de 30%,. O texto também concede perdão a irregularidades e abre um programa perpétuo de refinanciamento de débitos (Refis) para partidos políticos,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Projeto "Novo Cangaço"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A Câmara aprovou em votação simbólica um projeto que tipifica e torna crime hediondo o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>domínio de cidades</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> por criminosos armados. O texto estabelece penas que podem chegar a 40 anos para o crime.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Arcabouço Fiscal (Texto-base)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Foi aprovado o texto-base do novo arcabouço fiscal, que combina metas de resultado primário com um limite de crescimento para gastos,. A votação representou uma importante vitória para o governo Lula, recebendo 372 votos favoráveis e 108 contrários.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Arcabouço Fiscal (Gatilhos)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Parlamentares deram apoio expressivo (429 votos a 20) à inclusão de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gatilhos automáticos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> no arcabouço para ajustar despesas,. As medidas incluem a proibição de concursos públicos e de aumentos salariais para servidores em caso de descumprimento da meta fiscal,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Arcabouço Fiscal (Final)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: O Congresso Nacional, após o texto retornar do Senado, aprovou o novo arcabouço fiscal, pondo fim ao teto de gastos,. A Câmara aprovou blocos de emendas com 379 e 423 votos favoráveis, respectivamente, sendo o suficiente para o texto seguir para sanção presidencial,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Regulamentação de Apostas Esportivas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Foi aprovado o projeto de lei que regulamenta as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>apostas esportivas online</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ('bets') em votação simbólica. O governo esperava arrecadar R$ 1,6 bilhão em 2024 com a atividade.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Agenda de Costumes na LDO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: O Congresso aprovou, com 305 votos a 141 na Câmara, uma emenda na Lei de Diretrizes Orçamentárias (LDO) que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>impede a União de financiar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> invasão de terras e cirurgias de troca de sexo em crianças,,. O governo Lula, que sofreu uma derrota com a aprovação, prometeu vetar o trecho,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Política Nacional de Cuidado às Demências</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A Câmara aprovou a Política Nacional de Cuidado Integral às Pessoas com Doença de Alzheimer e Outras Demências. O projeto define diretrizes para o tratamento das doenças, aguardando sanção presidencial,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Taxação de Compras Internacionais (20%)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A Câmara aprovou a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>taxação de 20%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sobre compras internacionais de até US$ 50. Esta medida foi aprovada antes de ser definitivamente incorporada ao projeto Mover,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Taxa das Blusinhas (Mover)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A Câmara dos Deputados aprovou a taxação das compras internacionais de até US$ 50, a chamada "taxa das blusinhas", dentro do texto-base do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>projeto de lei do Mover</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,. A tributação para os produtos mais baratos será de 20% sobre o valor.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fiscalização de Concessionárias de Energia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Foi aprovado em votação simbólica um projeto de lei que permite que as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prefeituras fiscalizem a atuação de concessionárias</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de energia elétrica,. A discussão ganhou força após um apagão de larga escala em São Paulo,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Imposto Mínimo Global</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A Câmara dos Deputados aprovou o projeto que cria o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>imposto mínimo global</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de 15% sobre o lucro de empresas multinacionais,. A aprovação ocorreu um dia antes de o Senado manter o texto e enviá-lo à sanção presidencial.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Recursos do Pré-sal para Cotistas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A Câmara aprovou um projeto de lei que determina que parte do lucro do pré-sal seja destinado a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>políticas de permanência estudantil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> em universidades públicas, beneficiando cotistas,. O projeto visa combater a evasão de estudantes em situação de vulnerabilidade.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PEC da Blindagem/Prerrogativas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A Câmara aprovou em dois turnos a PEC que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>amplia as prerrogativas de deputados e senadores</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> em processos criminais,. A medida exige licença da Casa Legislativa para processar criminalmente parlamentares e restringe medidas cautelares,.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PL contra Resolução do Conanda (Aborto Legal)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A Câmara aprovou um projeto de decreto legislativo (PDL) para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>derrubar a resolução do Conanda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sobre diretrizes de aborto legal em crianças e adolescentes. O projeto recebeu 317 votos favoráveis e 111 contrários.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PL Antifacção</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: O chamado “PL Antifacção”, que promete ser a resposta do Estado ao crime organizado, foi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aprovado na Câmara dos Deputados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. O projeto eleva as penas, podendo chegar a 66 anos, e endurece a progressão de regime.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>Fim do DPVAT (Revogação)</t>
     </r>
     <r>
@@ -2529,1733 +4255,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Aprovada a emenda (444 votos a 16) que revoga a lei que havia recriado o seguro obrigatório DPVAT apenas sete meses antes,. A medida, incluída em um pacote de corte de gastos do governo, segue para análise do Senado,,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Pena para Imagens de Nudez Geradas por IA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Aprovado o projeto de lei que inclui no Código Penal o crime de manipular, produzir ou divulgar conteúdo de nudez ou ato sexual falso gerado por inteligência artificial,. O crime pode ser punido com reclusão de dois a seis anos e multa, com aumento de pena se a vítima for mulher, criança ou idosa.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Reajuste dos Servidores Públicos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Aprovado o reajuste para servidores públicos (388 a 43 votos), garantindo um impacto de R$ 17,9 bilhões em 2025 para os aumentos salariais,. A discussão sobre a reestruturação de carreiras (Sidec) foi postergada para um grupo de trabalho,,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Pauta-Bomba de Crédito Subsidiado para o Agronegócio</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Aprovado (346 a 93) um projeto que inclui um crédito subsidiado de até R$ 30 bilhões para o agronegócio, usando verbas do Fundo Social do pré-sal,,. A votação ocorreu em um clima de retaliação após decisões desfavoráveis do Executivo e Judiciário,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Flexibilização do Licenciamento Ambiental</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Aprovado o projeto (267 a 116) que flexibiliza e simplifica o licenciamento ambiental, mantendo mecanismos criticados por ambientalistas, como a Licença Ambiental Especial (LAE),,,. O texto, que segue para sanção presidencial, é visto como um impulso para projetos como a exploração de petróleo na Foz do Amazonas,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Proteção de Crianças e Adolescentes no Ambiente Digital</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Aprovado simbolicamente (apenas Novo e um deputado votaram contra) o projeto que visa proteger crianças e adolescentes em meios digitais, exigindo que plataformas implementem mecanismos para impedir acesso a conteúdos inadequados,,. O texto segue para o Senado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Criação do Sistema Nacional de Educação ('SUS da Educação')</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Aprovado o projeto que institui o Sistema Nacional de Educação (SNE), buscando a cooperação técnica e financeira entre União, estados e municípios para políticas educacionais,,. O texto cria a Infraestrutura Nacional de Dados da Educação e o Identificador Nacional Único do Estudante.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Gratuidade de Bagagem e Marcação de Assento</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Aprovada a gratuidade da bagagem despachada (361 a 77 votos) e de mão, além da proibição de cobrança pela marcação de assento padrão em voos nacionais ou internacionais,,. O projeto segue para o Senado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Medidas de Corte de Gastos e Atualização de Imóveis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Aprovado o projeto (286 a 146) que cria o Regime Especial de Atualização e Regularização Patrimonial (Rearp) de bens móveis e imóveis, com pagamento de alíquota menor de tributo,. O texto incluiu medidas de contenção de despesas do governo, com impacto fiscal estimado em R$ 15 bilhões,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Plano Nacional do Esporte (PNEsporte)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, previsto na Lei Pelé, que estabelece princípios e objetivos para o esporte brasileiro,,. O texto proíbe o contingenciamento de recursos destinados ao esporte provenientes da arrecadação das loterias federais,. A votação foi simbólica e a proposta seguiu para o Senado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Foi aprovada uma Medida Provisória (MP) que autoriza a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>concessão de empréstimo consignado</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> para beneficiários do Auxílio Brasil e do BPC (Benefício de Prestação Continuada),. O limite de contratação de crédito consignado para esses beneficiários é de 40% do valor do benefício,. O texto-base foi aprovado por 245 votos a 69.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou uma MP para </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>reduzir as filas do INSS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, permitindo a concessão de auxílio por incapacidade temporária (o antigo auxílio-doença) sem perícia médica presencial,. A MP também inclui o auxílio-acidente no rol de benefícios que passarão por reavaliações e revisões periódicas,. O texto-base foi aprovado por 381 votos a 8.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Foi aprovada uma Medida Provisória que autoriza o governo a adotar </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>medidas trabalhistas alternativas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (como teletrabalho facilitado e antecipação de férias) para mitigar as consequências sociais e econômicas de um estado de calamidade pública,. O texto-base foi aprovado por 249 votos a 111.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O texto-base da Medida Provisória que altera as regras sobre o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>vale-alimentação</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> foi aprovado por 248 votos a 159,. Uma das principais mudanças mantidas permite que, após 60 dias sem uso, o saldo do vale-alimentação possa ser sacado pelo trabalhador.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Foi aprovado o projeto que cria as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>loterias da Saúde e do Turismo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, permitindo a exploração dos novos jogos pela iniciativa privada,. Os recursos arrecadados serão destinados ao Fundo Nacional de Saúde (FNS) e à Embratur,. O texto foi aprovado por 267 a 94.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou em dois turnos uma PEC que permite a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>reeleição para a direção dos Tribunais de Justiça (TJs)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> estaduais que possuem mais de 170 desembargadores, o que se aplica aos TJs de São Paulo e Rio de Janeiro,,. A inclusão da possibilidade de recondução foi acrescentada ao texto um dia antes da votação, sem debate em comissões.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou uma MP do governo Bolsonaro que </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>afrouxa a proteção à Mata Atlântica</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">,. O texto, alterado pelo relator, flexibiliza o desmatamento de vegetação primária e secundária e retira a exigência de medidas compensatórias para supressão fora de Áreas de Preservação Permanente (APP),,. O plenário também aprovou uma outra MP que permite a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>comercialização de créditos de carbono</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> em concessões de unidades de conservação e florestas públicas,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O plenário aprovou o texto-base da MP que </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>reestrutura a Esplanada dos Ministérios</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, evitando uma derrota do governo Lula,. O texto amplia o número de ministérios para 37, mas o governo foi obrigado a ceder e aceitar a recriação da Funasa,. A aprovação teve 337 votos a favor e 125 contra.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou o projeto de lei que cria o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>programa Escola em Tempo Integral</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. A proposta, que segue ao Senado, prevê um investimento de R$ 2 bilhões em assistência financeira para 2023 e 2024, com o objetivo de viabilizar um milhão de novas matrículas,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O texto do projeto que prorroga a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>desoneração da folha de pagamento</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> para 17 setores da economia até 2027 foi aprovado, representando uma derrota dupla para o ministro Fernando Haddad (Fazenda),. O projeto também reduz a contribuição previdenciária de municípios,. Recebeu 430 votos favoráveis e 17 contrários.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Aprovado em votação simbólica o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PL do Desenrola Brasil</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, que estabelece regras para o programa de renegociação de dívidas e prevê um limite para os juros do rotativo do cartão de crédito,,. Caso as instituições financeiras não apresentem um plano de taxa menor em 90 dias, a dívida será limitada ao dobro do montante original,,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou o projeto que libera </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R$ 13,9 bilhões em repasses</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> para estados e municípios em 2023,. O montante inclui R$ 10 bilhões antecipados da compensação por cortes no ICMS e reposição de perdas nos fundos de participação (FPM e FPE),. O texto-base foi aprovado por 349 votos a 68.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O Congresso Nacional aprovou uma série de projetos para </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>realocar recursos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> entre ministérios, com o objetivo de aumentar verbas para pastas e projetos ligados ao centrão e vitaminar as emendas parlamentares,. O Ministério das Cidades e o do Desenvolvimento Social perderam recursos em favor de órgãos como Codevasf,,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>prorrogação da Lei Paulo Gustavo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> até dezembro de 2024, que destina R$ 3,86 bilhões para o fomento de atividades culturais,. A proposta seguiu para sanção presidencial e foi aprovada por 326 votos a 84,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou um projeto de lei que cria um </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cadastro nacional para monitorar facções criminosas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, incluindo milícias,. O cadastro será atualizado com base em decisões judiciais transitadas em julgado (condenações definitivas) e as informações reunidas serão sigilosas,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Foi aprovado o projeto de lei que </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>criminaliza a violação, adulteração ou troca de bagagem</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de passageiros de avião ou ônibus para fins de tráfico de drogas,. O crime terá pena de 5 a 15 anos, que pode ser aumentada se o agente for funcionário do serviço de transporte,. A votação foi simbólica.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou, de forma simbólica, um projeto de lei que cria uma </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>política de acolhimento de animais resgatados</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> durante desastres naturais,. A proposta prevê que municípios organizem sistemas de resgate e abrigos temporários, com equipes treinadas e avaliação veterinária imediata,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Em votação simbólica, foi aprovado o projeto de lei conhecido como "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lei Larissa Manoela</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", que insere no ECA (Estatuto da Criança e do Adolescente) o direito à proteção contra condutas abusivas na gestão patrimonial de crianças e adolescentes,,. O texto permite que um juiz determine restrições de acesso dos pais aos recursos ou a criação de uma reserva especial.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou um projeto que prorroga </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>benefícios tributários para o setor audiovisual</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (como o Recine e a Lei do Audiovisual) e autoriza a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>redução de repasses da Lei Aldir Blanc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> a estados e municípios que possuírem recursos não utilizados do ano anterior,,,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Foi aprovado o projeto de lei complementar que visa aumentar o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>número de deputados federais de 513 para 531</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,. O aumento cria 18 novas cadeiras para redistribuir a representação dos estados de acordo com o Censo 2022, evitando que algumas bancadas perdessem assentos,. O placar foi de 270 a favor e 207 contra.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou projeto de lei que </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aumenta as penas para crimes contra profissionais de saúde</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,. A proposta transforma em homicídio qualificado o assassinato desses profissionais no exercício da função (pena de 12 a 30 anos) e inclui lesão corporal contra eles no Código Penal (pena de 2 a 5 anos de prisão),. O texto foi aprovado por 310 votos contra 105.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Foi aprovado o projeto que institui a chamada </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Lei do Mar"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, estabelecendo a Política Nacional para a Gestão Integrada, a Conservação e o Uso Sustentável do Sistema Costeiro-Marinho (PNGCMar),. O texto foi aprovado com 376 votos a favor e 66 contrários após 12 anos de discussão.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>derrubada dos decretos do governo que aumentavam as alíquotas do IOF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Imposto sobre Operações Financeiras). A medida foi aprovada por 383 votos a 98.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Em votação a jato, a Câmara aprovou a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>redação final do projeto que aumenta o número de deputados</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de 513 para 531, incorporando alterações feitas pelo Senado,. As alterações incluíram uma restrição que proíbe qualquer aumento de despesa devido à criação das 18 novas cadeiras,. As mudanças tiveram o voto favorável de 361 deputados, contra 33.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou o projeto de lei que </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dificulta a progressão de pena</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> para condenados por crimes hediondos (como estupro e homicídio), exigindo o cumprimento de, no mínimo, 80% da pena,,. A regra também se aplica a sentenciados por constituir milícia privada ou exercer comando em organização criminosa.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Em dois turnos (446 a 20 e 426 a 10), a Câmara aprovou uma PEC que </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>afrouxa as regras de aposentadoria para agentes comunitários de saúde e de combate a endemias</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,,. A medida, apelidada de "contrarreforma da Previdência", restabelece a integralidade e a paridade para a categoria, com um potencial impacto bilionário (estimado entre R$ 20 bilhões e R$ 200 bilhões) nas contas da União,,,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Foi aprovado um pacote de 16 projetos relacionados à infância e educação. Entre eles, um projeto </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aumenta a pena para pedófilos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (ex: estupro de vulnerável de 8-15 para 10-18 anos) e outro exige </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>autorização judicial para a atividade de influenciadores mirins</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou dois projetos propostos pelo STF para </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aumentar os salários dos servidores do Poder Judiciário</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> da União,. Um reajusta em 25,97% os vencimentos (escalonado até 2028), com 299 votos a 119. O outro, aprovado simbolicamente, ajusta o adicional de qualificação baseado em cursos e pós-graduação.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ratificação do Acordo de Escazú</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, um tratado internacional sobre transparência, participação pública, segurança e justiça em temas ambientais,. O acordo estava engavetado há seis anos e foi aprovado na véspera da COP30,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou um projeto de lei que institui a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Política Nacional de Saúde Masculina no SUS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, com foco em prevenção, detecção precoce e tratamento de doenças que acometem os homens,. O texto também implementa a campanha Novembro Azul em nível nacional.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou a versão do relator Guilherme Derrite (PP-SP) para o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PL Antifacção</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, em uma derrota para o governo Lula que tentava adiar a apreciação,. O projeto cria novos tipos penais, como Domínio Social Estruturado, para endurecer a punição contra organizações criminosas ultraviolentas,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou o projeto de lei que </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>prorroga a lei de cotas para negros em concursos públicos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,. O texto aumenta a reserva de vagas de 20% para 30% e inclui indígenas e quilombolas entre os beneficiados, mas precisará retornar ao Senado devido às alterações,,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou a MP que liberou </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>crédito extraordinário de R$ 12 bilhões</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> para ações de socorro ao Rio Grande do Sul em decorrência das enchentes,. O texto foi aprovado com 257 votos favoráveis e 150 contrários.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Foi aprovada a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lei Geral do Turismo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, retirando o trecho polêmico que limitaria a indenização a passageiros de companhias aéreas,,. O texto permite, entre outras coisas, a reabertura de empréstimos garantidos pelo Fundo Nacional da Aviação Civil (Fnac) para companhias aéreas.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou uma alteração na </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lei de Responsabilidade Fiscal (LRF)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> que flexibiliza os limites de gasto com pessoal de estados e municípios,. A mudança permite descontar do cálculo de despesa com pessoal os gastos com terceirização e organizações da sociedade civil,. A proposta foi aprovada por 370 votos favoráveis contra 15.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou um projeto que dá maior </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fôlego orçamentário a hospitais universitários</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. A medida exclui despesas de pessoal desses hospitais do cálculo para o cumprimento do limite constitucional mínimo de aplicação anual em saúde pública,. O texto será enviado à sanção presidencial.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara concluiu a votação e aprovou a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>desoneração da folha de pagamento</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> para 17 setores e municípios, após impasse com o Banco Central,. O projeto, aprovado por 253 votos a favor, mantém o benefício em 2024 e estabelece uma reoneração gradual entre 2025 e 2027,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou o projeto de lei que exige que as empresas aéreas </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ofereçam o serviço de rastreamento de animais de estimação (pets)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> transportados em voos domésticos,,. A proposta, aprovada de forma simbólica, surge após a morte do cão Joca,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Foi aprovado o projeto de lei que cria </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R$ 18,3 bilhões em subsídios fiscais para projetos de hidrogênio verde</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,. O texto, que segue para o Senado, foi negociado após um veto anterior do presidente Lula, e concede crédito fiscal por meio da Contribuição Social sobre o Lucro Líquido (CSLL),,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A Câmara aprovou, em dois turnos (344 a 89 e 338 a 83), a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PEC da Anistia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. A proposta revoga a obrigatoriedade de distribuir verba eleitoral de forma proporcional ao número de candidatos negros (pretos e pardos), fixando um mínimo de 30%,. O texto também concede perdão a irregularidades e abre um programa perpétuo de refinanciamento de débitos (Refis) para partidos políticos,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Projeto "Novo Cangaço"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: A Câmara aprovou em votação simbólica um projeto que tipifica e torna crime hediondo o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>domínio de cidades</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> por criminosos armados. O texto estabelece penas que podem chegar a 40 anos para o crime.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Arcabouço Fiscal (Texto-base)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Foi aprovado o texto-base do novo arcabouço fiscal, que combina metas de resultado primário com um limite de crescimento para gastos,. A votação representou uma importante vitória para o governo Lula, recebendo 372 votos favoráveis e 108 contrários.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Arcabouço Fiscal (Gatilhos)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Parlamentares deram apoio expressivo (429 votos a 20) à inclusão de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>gatilhos automáticos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> no arcabouço para ajustar despesas,. As medidas incluem a proibição de concursos públicos e de aumentos salariais para servidores em caso de descumprimento da meta fiscal,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Arcabouço Fiscal (Final)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: O Congresso Nacional, após o texto retornar do Senado, aprovou o novo arcabouço fiscal, pondo fim ao teto de gastos,. A Câmara aprovou blocos de emendas com 379 e 423 votos favoráveis, respectivamente, sendo o suficiente para o texto seguir para sanção presidencial,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Regulamentação de Apostas Esportivas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Foi aprovado o projeto de lei que regulamenta as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>apostas esportivas online</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ('bets') em votação simbólica. O governo esperava arrecadar R$ 1,6 bilhão em 2024 com a atividade.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Agenda de Costumes na LDO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: O Congresso aprovou, com 305 votos a 141 na Câmara, uma emenda na Lei de Diretrizes Orçamentárias (LDO) que </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>impede a União de financiar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> invasão de terras e cirurgias de troca de sexo em crianças,,. O governo Lula, que sofreu uma derrota com a aprovação, prometeu vetar o trecho,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Política Nacional de Cuidado às Demências</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: A Câmara aprovou a Política Nacional de Cuidado Integral às Pessoas com Doença de Alzheimer e Outras Demências. O projeto define diretrizes para o tratamento das doenças, aguardando sanção presidencial,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Taxação de Compras Internacionais (20%)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: A Câmara aprovou a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>taxação de 20%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sobre compras internacionais de até US$ 50. Esta medida foi aprovada antes de ser definitivamente incorporada ao projeto Mover,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Taxa das Blusinhas (Mover)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: A Câmara dos Deputados aprovou a taxação das compras internacionais de até US$ 50, a chamada "taxa das blusinhas", dentro do texto-base do </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>projeto de lei do Mover</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,. A tributação para os produtos mais baratos será de 20% sobre o valor.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Fiscalização de Concessionárias de Energia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Foi aprovado em votação simbólica um projeto de lei que permite que as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>prefeituras fiscalizem a atuação de concessionárias</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de energia elétrica,. A discussão ganhou força após um apagão de larga escala em São Paulo,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Imposto Mínimo Global</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: A Câmara dos Deputados aprovou o projeto que cria o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>imposto mínimo global</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de 15% sobre o lucro de empresas multinacionais,. A aprovação ocorreu um dia antes de o Senado manter o texto e enviá-lo à sanção presidencial.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Recursos do Pré-sal para Cotistas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: A Câmara aprovou um projeto de lei que determina que parte do lucro do pré-sal seja destinado a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>políticas de permanência estudantil</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> em universidades públicas, beneficiando cotistas,. O projeto visa combater a evasão de estudantes em situação de vulnerabilidade.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PEC da Blindagem/Prerrogativas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: A Câmara aprovou em dois turnos a PEC que </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>amplia as prerrogativas de deputados e senadores</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> em processos criminais,. A medida exige licença da Casa Legislativa para processar criminalmente parlamentares e restringe medidas cautelares,.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PL contra Resolução do Conanda (Aborto Legal)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: A Câmara aprovou um projeto de decreto legislativo (PDL) para </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>derrubar a resolução do Conanda</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sobre diretrizes de aborto legal em crianças e adolescentes. O projeto recebeu 317 votos favoráveis e 111 contrários.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PL Antifacção</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: O chamado “PL Antifacção”, que promete ser a resposta do Estado ao crime organizado, foi </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aprovado na Câmara dos Deputados</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. O projeto eleva as penas, podendo chegar a 66 anos, e endurece a progressão de regime.</t>
+      <t xml:space="preserve"> Aprovada a emenda (444 votos a 16) que revoga a lei que havia recriado o seguro obrigatório DPVAT apenas sete meses antes,. A medida, incluída em um pacote de corte de gastos do governo, segue para análise do Senado (PROJETO É SOBRE LIMITE DE DESPESAS E INCLUI O ASSUNTO DPVAT; CRIEI VOTEBEM PARCIAL)</t>
     </r>
   </si>
 </sst>
@@ -4288,12 +4288,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4308,7 +4326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4318,6 +4336,21 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4636,8 +4669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77711C5D-96D0-4B88-B71E-5764725EFA53}">
   <dimension ref="A1:D1429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4694,7 +4727,7 @@
       <c r="A7" s="4">
         <v>46001</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C7" s="2"/>
@@ -4703,8 +4736,8 @@
       <c r="A8" s="4">
         <v>45980</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>363</v>
+      <c r="B8" s="8" t="s">
+        <v>362</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -4712,8 +4745,8 @@
       <c r="A9" s="4">
         <v>45979</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>339</v>
+      <c r="B9" s="7" t="s">
+        <v>338</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -4721,8 +4754,8 @@
       <c r="A10" s="4">
         <v>45972</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>338</v>
+      <c r="B10" s="6" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
@@ -4730,15 +4763,15 @@
         <v>45966</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A12" s="4">
         <v>45966</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>362</v>
+      <c r="B12" s="8" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
@@ -4746,7 +4779,7 @@
         <v>45965</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
@@ -4754,14 +4787,14 @@
         <v>45959</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A15" s="4">
         <v>45958</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>261</v>
       </c>
     </row>
@@ -4770,15 +4803,15 @@
         <v>45958</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A17" s="4">
         <v>45945</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>335</v>
+      <c r="B17" s="6" t="s">
+        <v>334</v>
       </c>
       <c r="C17" s="2"/>
     </row>
@@ -4794,15 +4827,15 @@
       <c r="A19" s="4">
         <v>45937</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>334</v>
+      <c r="B19" s="7" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A20" s="4">
         <v>45931</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="8" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4810,7 +4843,7 @@
       <c r="A21" s="4">
         <v>45931</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="7" t="s">
         <v>260</v>
       </c>
     </row>
@@ -4818,7 +4851,7 @@
       <c r="A22" s="4">
         <v>45924</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="8" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4826,7 +4859,7 @@
       <c r="A23" s="4">
         <v>45924</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="7" t="s">
         <v>259</v>
       </c>
     </row>
@@ -4834,24 +4867,24 @@
       <c r="A24" s="4">
         <v>45916</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>361</v>
+      <c r="B24" s="8" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A25" s="4">
         <v>45903</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>305</v>
+      <c r="B25" s="8" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A26" s="4">
         <v>45889</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>304</v>
+      <c r="B26" s="5" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
@@ -4866,23 +4899,23 @@
       <c r="A28" s="4">
         <v>45855</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>303</v>
+      <c r="B28" s="5" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A29" s="4">
         <v>45854</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>302</v>
+      <c r="B29" s="8" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A30" s="4">
         <v>45847</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="5" t="s">
         <v>230</v>
       </c>
     </row>
@@ -4890,8 +4923,8 @@
       <c r="A31" s="4">
         <v>45840</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>333</v>
+      <c r="B31" s="7" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
@@ -4899,39 +4932,39 @@
         <v>45833</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A33" s="4">
         <v>45833</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>332</v>
+      <c r="B33" s="7" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A34" s="4">
         <v>45833</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>360</v>
+      <c r="B34" s="5" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A35" s="4">
         <v>45804</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>329</v>
+      <c r="B35" s="6" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A36" s="4">
         <v>45804</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>330</v>
+      <c r="B36" s="7" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -4939,54 +4972,54 @@
         <v>45798</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A38" s="4">
         <v>45783</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>328</v>
+      <c r="B38" s="7" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A39" s="4">
         <v>45775</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>327</v>
+      <c r="B39" s="7" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A40" s="4">
         <v>45741</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>326</v>
+      <c r="B40" s="6" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A41" s="4">
         <v>45707</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>300</v>
+      <c r="B41" s="5" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A42" s="4">
         <v>45693</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>325</v>
+      <c r="B42" s="6" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A43" s="4">
         <v>45644</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="8" t="s">
         <v>229</v>
       </c>
     </row>
@@ -4994,23 +5027,23 @@
       <c r="A44" s="4">
         <v>45644</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="6" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A45" s="4">
         <v>45644</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>299</v>
+      <c r="B45" s="9" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A46" s="4">
         <v>45643</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="6" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5018,7 +5051,7 @@
       <c r="A47" s="4">
         <v>45643</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="5" t="s">
         <v>298</v>
       </c>
     </row>
@@ -5026,8 +5059,8 @@
       <c r="A48" s="4">
         <v>45643</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>359</v>
+      <c r="B48" s="5" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5043,7 +5076,7 @@
         <v>45636</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5051,7 +5084,7 @@
         <v>45636</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5091,7 +5124,7 @@
         <v>45615</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5147,7 +5180,7 @@
         <v>45582</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5163,7 +5196,7 @@
         <v>45547</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5179,7 +5212,7 @@
         <v>45545</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5195,7 +5228,7 @@
         <v>45532</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5203,7 +5236,7 @@
         <v>45532</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5211,7 +5244,7 @@
         <v>45530</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5227,7 +5260,7 @@
         <v>45516</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5243,7 +5276,7 @@
         <v>45484</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5283,7 +5316,7 @@
         <v>45454</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5299,7 +5332,7 @@
         <v>45440</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5347,7 +5380,7 @@
         <v>45420</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5355,7 +5388,7 @@
         <v>45420</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5411,7 +5444,7 @@
         <v>45279</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5435,7 +5468,7 @@
         <v>45260</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5491,7 +5524,7 @@
         <v>45203</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5507,7 +5540,7 @@
         <v>45183</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5523,7 +5556,7 @@
         <v>45182</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5539,7 +5572,7 @@
         <v>45174</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5547,7 +5580,7 @@
         <v>45168</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5555,7 +5588,7 @@
         <v>45160</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5587,7 +5620,7 @@
         <v>45110</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5611,7 +5644,7 @@
         <v>45077</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5627,7 +5660,7 @@
         <v>45070</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5635,7 +5668,7 @@
         <v>45069</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5651,7 +5684,7 @@
         <v>45015</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5715,7 +5748,7 @@
         <v>44874</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5731,7 +5764,7 @@
         <v>44803</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5779,7 +5812,7 @@
         <v>44776</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5787,7 +5820,7 @@
         <v>44776</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5795,7 +5828,7 @@
         <v>44775</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5803,7 +5836,7 @@
         <v>44775</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
@@ -5835,7 +5868,7 @@
         <v>44741</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5843,7 +5876,7 @@
         <v>44740</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
pagina exclusiva para divulgadores, passo 1
</commit_message>
<xml_diff>
--- a/docs/Noticias/Resumo votações na Câmara.xlsx
+++ b/docs/Noticias/Resumo votações na Câmara.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dados\Tecnicos\HardESoftware\EmDesenvolvimento\VotoBomPython\django_votebem\docs\Noticias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F228F416-87CC-4A38-8BE7-70630A341FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3501A94C-3A07-47CF-8AF9-2C36AED17EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{53B4B6C9-9AD8-4847-8B7A-A3110067C019}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="368">
   <si>
     <t>Votações Aprovadas na Câmara dos Deputados</t>
   </si>
@@ -4257,13 +4257,32 @@
       </rPr>
       <t xml:space="preserve"> Aprovada a emenda (444 votos a 16) que revoga a lei que havia recriado o seguro obrigatório DPVAT apenas sete meses antes,. A medida, incluída em um pacote de corte de gastos do governo, segue para análise do Senado (PROJETO É SOBRE LIMITE DE DESPESAS E INCLUI O ASSUNTO DPVAT; CRIEI VOTEBEM PARCIAL)</t>
     </r>
+  </si>
+  <si>
+    <t>Câmara dos Deputados decide manter prisão de Chiquinho Brazão, 277 a 129
+Parlamentar está preso desde março por determinação de Alexandre de Moraes, do Supremo Tribunal Federal. Ele é um dos suspeitos de mandar matar a vereadora Marielle Franco, em 2018
+https://www.nexojornal.com.br/extra/2024/04/10/decisao-da-camara-chiquinho-brazao</t>
+  </si>
+  <si>
+    <t>https://www.nexojornal.com.br/extra/2022/07/13/camara-aprova-pec-que-garante-piso-salarial-para-enfermagem
+Câmara aprova PEC que garante piso salarial para enfermagem, 473 x 9
+Medida ampara projeto de lei federal que institui remuneração mínima para enfermeiros, técnicos, auxiliares e parteiras</t>
+  </si>
+  <si>
+    <t>Câmara aprova PEC das bondades às vésperas das eleições
+https://www.nexojornal.com.br/extra/2022/07/12/camara-aprova-pec-das-bondades-as-vesperas-das-eleicoes</t>
+  </si>
+  <si>
+    <t>Câmara aprova projeto que limita ICMS sobre combustíveis
+Medida pode forçar estados a reduzirem alíquotas e perderem receita. Proposta segue para o Senado, onde governadores tentarão impedir a aprovação
+https://www.nexojornal.com.br/extra/2022/05/26/camara-aprova-projeto-que-limita-icms-sobre-combustiveis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4283,6 +4302,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4323,10 +4350,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4353,8 +4381,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4667,10 +4705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77711C5D-96D0-4B88-B71E-5764725EFA53}">
-  <dimension ref="A1:D1429"/>
+  <dimension ref="A1:D1433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -5399,12 +5437,12 @@
         <v>290</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:2" ht="59" x14ac:dyDescent="0.75">
       <c r="A91" s="4">
-        <v>45391</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>246</v>
+        <v>45392</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5412,79 +5450,79 @@
         <v>45391</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A93" s="4">
         <v>45391</v>
       </c>
-      <c r="B93" s="3" t="s">
-        <v>289</v>
+      <c r="B93" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A94" s="4">
-        <v>45371</v>
+        <v>45391</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A95" s="4">
         <v>45371</v>
       </c>
       <c r="B95" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A96" s="4">
+        <v>45371</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A96" s="4">
+    <row r="97" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A97" s="4">
         <v>45279</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>353</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A97" s="4">
-        <v>45273</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A98" s="4">
+        <v>45273</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A99" s="4">
         <v>45266</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A99" s="4">
-        <v>45260</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A100" s="4">
-        <v>45259</v>
+        <v>45260</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>245</v>
+        <v>321</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A101" s="4">
         <v>45259</v>
       </c>
-      <c r="B101" s="3" t="s">
-        <v>283</v>
+      <c r="B101" s="2" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5492,47 +5530,47 @@
         <v>45259</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A103" s="4">
-        <v>45252</v>
+        <v>45259</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A104" s="4">
-        <v>45230</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>244</v>
+        <v>45252</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A105" s="4">
-        <v>45224</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>281</v>
+        <v>45230</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A106" s="4">
-        <v>45203</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>320</v>
+        <v>45224</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A107" s="4">
-        <v>45183</v>
+        <v>45203</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>243</v>
+        <v>320</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5540,15 +5578,15 @@
         <v>45183</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>319</v>
+        <v>243</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A109" s="4">
-        <v>45182</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>280</v>
+        <v>45183</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5556,223 +5594,223 @@
         <v>45182</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>352</v>
+        <v>280</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A111" s="4">
+        <v>45182</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A112" s="4">
         <v>45181</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A112" s="4">
+    <row r="113" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A113" s="4">
         <v>45174</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>318</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A113" s="4">
-        <v>45168</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A114" s="4">
-        <v>45160</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>351</v>
+        <v>45168</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A115" s="4">
+        <v>45160</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A116" s="4">
         <v>45153</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A116" s="4">
-        <v>45147</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A117" s="4">
+        <v>45147</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A118" s="4">
         <v>45114</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A118" s="4">
-        <v>45110</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A119" s="4">
-        <v>45091</v>
+        <v>45110</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A120" s="4">
         <v>45091</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A121" s="4">
+        <v>45091</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A121" s="4">
-        <v>45077</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A122" s="4">
-        <v>45076</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>275</v>
+        <v>45077</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A123" s="4">
-        <v>45070</v>
+        <v>45076</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>350</v>
+        <v>275</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A124" s="4">
+        <v>45070</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A125" s="4">
         <v>45069</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B125" s="3" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A125" s="4">
-        <v>45049</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A126" s="4">
+        <v>45049</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A127" s="4">
         <v>45015</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B127" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A127" s="4">
+    <row r="128" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A128" s="4">
         <v>45007</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B128" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A128" s="4">
+    <row r="129" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A129" s="4">
         <v>44986</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B129" s="3" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A129" s="4">
-        <v>44916</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A130" s="4">
-        <v>44915</v>
+        <v>44916</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A131" s="4">
-        <v>44910</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>217</v>
+        <v>44915</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A132" s="4">
-        <v>44909</v>
+        <v>44910</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>273</v>
+        <v>217</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A133" s="4">
+        <v>44909</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A134" s="4">
         <v>44888</v>
       </c>
-      <c r="B133" s="3" t="s">
+      <c r="B134" s="3" t="s">
         <v>272</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A134" s="4">
-        <v>44874</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A135" s="4">
-        <v>44803</v>
+        <v>44874</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A136" s="4">
         <v>44803</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>312</v>
+        <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A137" s="4">
-        <v>44777</v>
+        <v>44803</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>237</v>
+        <v>312</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
@@ -5780,245 +5818,221 @@
         <v>44777</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A139" s="4">
-        <v>44776</v>
+        <v>44777</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A140" s="4">
         <v>44776</v>
       </c>
-      <c r="B140" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="B140" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A141" s="4">
         <v>44776</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A142" s="4">
         <v>44776</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>311</v>
+      <c r="B142" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A143" s="4">
         <v>44776</v>
       </c>
-      <c r="B143" s="3" t="s">
+      <c r="B143" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A144" s="4">
+        <v>44776</v>
+      </c>
+      <c r="B144" s="3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A144" s="4">
-        <v>44775</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A145" s="4">
         <v>44775</v>
       </c>
       <c r="B145" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A146" s="4">
+        <v>44775</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A146" s="4">
-        <v>44755</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A147" s="4">
         <v>44755</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B147" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A148" s="4">
+        <v>44755</v>
+      </c>
+      <c r="B148" s="12" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A149" s="4">
+        <v>44755</v>
+      </c>
+      <c r="B149" s="3" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A148" s="4">
-        <v>44748</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A149" s="4">
-        <v>44741</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A150" s="4">
-        <v>44740</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+        <v>44754</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A151" s="4">
-        <v>44726</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>268</v>
+        <v>44748</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A152" s="4">
-        <v>44720</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+        <v>44741</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A153" s="4">
-        <v>44719</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+        <v>44740</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A154" s="4">
-        <v>44713</v>
+        <v>44726</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A155" s="4">
-        <v>44699</v>
+        <v>44720</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A156" s="4">
+        <v>44719</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A157" s="4">
+        <v>44713</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="59" x14ac:dyDescent="0.75">
+      <c r="A158" s="4">
+        <v>44707</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A159" s="4">
+        <v>44699</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A160" s="4">
         <v>44692</v>
       </c>
-      <c r="B156" s="3" t="s">
+      <c r="B160" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A157" s="4">
+    <row r="161" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A161" s="4">
         <v>44678</v>
       </c>
-      <c r="B157" s="3" t="s">
+      <c r="B161" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="1358" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A1358" s="1" t="s">
+    <row r="1362" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A1362" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="1360" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A1360" s="3" t="s">
+    <row r="1364" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A1364" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1360" s="3" t="s">
+      <c r="B1364" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1360" s="3" t="s">
+      <c r="C1364" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1360" s="3" t="s">
+      <c r="D1364" s="3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="1361" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A1361" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1361" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1361" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1361" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1362" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A1362" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1362" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1362" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1362" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="1363" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A1363" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1363" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1363" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1363" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="1364" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A1364" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1364" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1364" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1364" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="1365" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1365" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B1365" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C1365" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D1365" s="2" t="s">
         <v>8</v>
@@ -6026,69 +6040,69 @@
     </row>
     <row r="1366" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1366" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B1366" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C1366" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D1366" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1367" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1367" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B1367" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C1367" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D1367" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1368" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1368" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B1368" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C1368" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D1368" s="2" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1369" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1369" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B1369" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C1369" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D1369" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1370" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1370" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B1370" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C1370" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D1370" s="2" t="s">
         <v>8</v>
@@ -6096,27 +6110,27 @@
     </row>
     <row r="1371" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1371" s="3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B1371" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C1371" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D1371" s="2" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1372" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1372" s="3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B1372" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C1372" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D1372" s="2" t="s">
         <v>31</v>
@@ -6124,13 +6138,13 @@
     </row>
     <row r="1373" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1373" s="3" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B1373" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C1373" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D1373" s="2" t="s">
         <v>12</v>
@@ -6138,111 +6152,111 @@
     </row>
     <row r="1374" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1374" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B1374" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C1374" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D1374" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1375" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1375" s="3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B1375" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C1375" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D1375" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1376" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1376" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B1376" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C1376" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D1376" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1377" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1377" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B1377" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C1377" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D1377" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1378" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1378" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B1378" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C1378" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D1378" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1379" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1379" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B1379" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C1379" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D1379" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1380" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1380" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B1380" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C1380" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1380" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1381" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1381" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B1381" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C1381" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D1381" s="2" t="s">
         <v>16</v>
@@ -6250,237 +6264,237 @@
     </row>
     <row r="1382" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1382" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B1382" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C1382" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D1382" s="2" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1383" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1383" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B1383" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C1383" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D1383" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1384" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1384" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B1384" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C1384" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D1384" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1385" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1385" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B1385" s="2" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C1385" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D1385" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1386" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1386" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B1386" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C1386" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D1386" s="2" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1387" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1387" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B1387" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C1387" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D1387" s="2" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1388" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1388" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B1388" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C1388" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D1388" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1389" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1389" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B1389" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C1389" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D1389" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1390" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1390" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B1390" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C1390" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D1390" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1391" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1391" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B1391" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C1391" s="2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D1391" s="2" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1392" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1392" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B1392" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C1392" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D1392" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1393" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1393" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B1393" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C1393" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D1393" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1394" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1394" s="3" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B1394" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C1394" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D1394" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1395" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1395" s="3" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B1395" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C1395" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D1395" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1396" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1396" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B1396" s="2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C1396" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D1396" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1397" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1397" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B1397" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C1397" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D1397" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1398" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1398" s="3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B1398" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C1398" s="2" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D1398" s="2" t="s">
         <v>12</v>
@@ -6488,237 +6502,237 @@
     </row>
     <row r="1399" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1399" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B1399" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C1399" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D1399" s="2" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1400" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1400" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B1400" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C1400" s="2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D1400" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1401" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1401" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B1401" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C1401" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D1401" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1402" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1402" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B1402" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C1402" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D1402" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1403" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1403" s="3" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B1403" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C1403" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D1403" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1404" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1404" s="3" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B1404" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C1404" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D1404" s="2" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1405" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1405" s="3" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B1405" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C1405" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D1405" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1406" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1406" s="3" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B1406" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C1406" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D1406" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1407" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1407" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B1407" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C1407" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D1407" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1408" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1408" s="3" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B1408" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C1408" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D1408" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1409" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1409" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B1409" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C1409" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="D1409" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1410" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1410" s="3" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B1410" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C1410" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D1410" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1411" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1411" s="3" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B1411" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C1411" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D1411" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1412" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1412" s="3" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="B1412" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C1412" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D1412" s="2" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1413" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1413" s="3" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B1413" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C1413" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D1413" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1414" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1414" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B1414" s="2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C1414" s="2" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D1414" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="1415" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1415" s="3" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B1415" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C1415" s="2" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D1415" s="2" t="s">
         <v>31</v>
@@ -6726,205 +6740,265 @@
     </row>
     <row r="1416" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1416" s="3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B1416" s="2" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C1416" s="2" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D1416" s="2" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1417" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1417" s="3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B1417" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C1417" s="2" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D1417" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1418" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1418" s="3" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B1418" s="2" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C1418" s="2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D1418" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="1419" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A1419" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B1419" s="2" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C1419" s="2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D1419" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1420" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1420" s="3" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B1420" s="2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C1420" s="2" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D1420" s="2" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1421" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1421" s="3" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B1421" s="2" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C1421" s="2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D1421" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1422" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1422" s="3" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B1422" s="2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C1422" s="2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="D1422" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1423" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1423" s="3" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B1423" s="2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C1423" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="D1423" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1424" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1424" s="3" t="s">
-        <v>13</v>
+        <v>180</v>
       </c>
       <c r="B1424" s="2" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C1424" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D1424" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A1425" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1425" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1425" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1425" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="1425" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A1425" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1425" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C1425" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D1425" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="1426" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1426" s="3" t="s">
-        <v>13</v>
+        <v>186</v>
       </c>
       <c r="B1426" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C1426" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D1426" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1427" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1427" s="3" t="s">
-        <v>19</v>
+        <v>189</v>
       </c>
       <c r="B1427" s="2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C1427" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D1427" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1428" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1428" s="3" t="s">
-        <v>200</v>
+        <v>13</v>
       </c>
       <c r="B1428" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C1428" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D1428" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1429" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A1429" s="3" t="s">
-        <v>203</v>
+        <v>13</v>
       </c>
       <c r="B1429" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C1429" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D1429" s="2" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="1430" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A1430" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1430" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1430" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1430" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A1431" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1431" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1431" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1431" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A1432" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1432" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1432" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1432" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A1433" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1433" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1433" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1433" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C157">
-    <sortCondition descending="1" ref="A4:A157"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C161">
+    <sortCondition descending="1" ref="A4:A161"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="B148" r:id="rId1" display="https://www.nexojornal.com.br/extra/2022/07/13/camara-aprova-pec-que-garante-piso-salarial-para-enfermagem_x000a_Câmara aprova PEC que garante piso salarial para enfermagem, 473 x 9_x000a_Medida ampara projeto de lei federal que institui remuneração mínima para enfermeiros, técnicos, auxiliares e parteiras" xr:uid="{D18DC7ED-B53E-4C5A-8BB4-E8D093F58EF6}"/>
+    <hyperlink ref="B158" r:id="rId2" display="https://www.nexojornal.com.br/extra/2022/05/26/camara-aprova-projeto-que-limita-icms-sobre-combustiveis" xr:uid="{4235241C-0647-460F-9087-B3A0EE6D7287}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>